<commit_message>
Remoção de alguns prints
</commit_message>
<xml_diff>
--- a/heroes enemy.xlsx
+++ b/heroes enemy.xlsx
@@ -4376,7 +4376,7 @@
         <v>1.0</v>
       </c>
       <c r="C29" s="4">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D29" s="4">
         <v>1.0</v>
@@ -4388,7 +4388,7 @@
         <v>0.0</v>
       </c>
       <c r="G29" s="4">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="H29" s="4">
         <v>0.0</v>
@@ -4397,7 +4397,7 @@
         <v>1.0</v>
       </c>
       <c r="J29" s="4">
-        <v>-1.0</v>
+        <v>-2.0</v>
       </c>
       <c r="K29" s="4">
         <v>0.0</v>
@@ -4448,7 +4448,7 @@
         <v>0.0</v>
       </c>
       <c r="AA29" s="4">
-        <v>-1.0</v>
+        <v>-2.0</v>
       </c>
       <c r="AB29" s="4">
         <v>0.0</v>

</xml_diff>